<commit_message>
made it calculate the hardness ratio and error for both instrustments for all bursts
</commit_message>
<xml_diff>
--- a/fermi_known_precursors_list.xlsx
+++ b/fermi_known_precursors_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nnuessle/Documents/Work/burst_matching_algorithm/actual_paper/prompt-and-afterglow-matching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1911E604-1C90-E048-A343-82627BFFC667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF385437-BB31-9043-A2F2-2F757BA164B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2240" windowWidth="30420" windowHeight="16940" xr2:uid="{415A39E4-12E1-0D46-96F2-16C855D612ED}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table!$A$1:$A$1</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Table!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -283,7 +283,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yymmddhhmmss"/>
+    <numFmt numFmtId="164" formatCode="yymmddhhmmss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -380,21 +380,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,13 +706,13 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D43"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -740,1128 +734,931 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="6">
         <v>38458.461626018521</v>
       </c>
-      <c r="C2" s="1" t="str">
+      <c r="C2" t="str">
         <f t="shared" ref="C2:C38" si="0">LEFT(RIGHT(B2,LEN(B2)-FIND(".",B2)),3)</f>
         <v>461</v>
       </c>
-      <c r="D2" s="7" t="str">
+      <c r="D2" t="str">
         <f t="shared" ref="D2:D38" si="1">_xlfn.CONCAT(LEFT(A2,LEN(A2)-1), C2)</f>
         <v>GRB050416461</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="6">
         <v>44069.187407407408</v>
       </c>
-      <c r="G2" s="1" t="str">
+      <c r="G2" t="str">
         <f t="shared" ref="G2" si="2">LEFT(RIGHT(F2,LEN(F2)-FIND(".",F2)),3)</f>
         <v>187</v>
       </c>
-      <c r="H2" s="7" t="str">
+      <c r="H2" t="str">
         <f t="shared" ref="H2" si="3">_xlfn.CONCAT(LEFT(E2,LEN(E2)-1), G2)</f>
         <v>GRB200826187</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="6">
         <v>39303.807141203702</v>
       </c>
-      <c r="K2" s="1" t="str">
+      <c r="K2" t="str">
         <f t="shared" ref="K2:K8" si="4">LEFT(RIGHT(J2,LEN(J2)-FIND(".",J2)),3)</f>
         <v>807</v>
       </c>
-      <c r="L2" s="7" t="str">
+      <c r="L2" t="str">
         <f>_xlfn.CONCAT(LEFT(I2,LEN(I2)), K2)</f>
         <v>GRB070809807</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="6">
         <v>38882.530416666668</v>
       </c>
-      <c r="O2" s="1" t="str">
+      <c r="O2" t="str">
         <f t="shared" ref="O2:O6" si="5">LEFT(RIGHT(N2,LEN(N2)-FIND(".",N2)),3)</f>
         <v>530</v>
       </c>
-      <c r="P2" s="7" t="str">
+      <c r="P2" t="str">
         <f>_xlfn.CONCAT(LEFT(M2,LEN(M2)), O2)</f>
         <v>GRB060614530</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="11">
+      <c r="R2" s="6">
         <v>44381.814867939815</v>
       </c>
-      <c r="S2" s="1" t="str">
+      <c r="S2" t="str">
         <f t="shared" ref="S2" si="6">LEFT(RIGHT(R2,LEN(R2)-FIND(".",R2)),3)</f>
         <v>814</v>
       </c>
-      <c r="T2" s="7" t="str">
+      <c r="T2" t="str">
         <f t="shared" ref="T2" si="7">_xlfn.CONCAT(LEFT(Q2,LEN(Q2)-1), S2)</f>
         <v>GRB210704814</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="6">
         <v>38497.002002314817</v>
       </c>
-      <c r="C3" s="1" t="str">
+      <c r="C3" t="str">
         <f t="shared" si="0"/>
         <v>002</v>
       </c>
-      <c r="D3" s="7" t="str">
+      <c r="D3" t="str">
         <f t="shared" si="1"/>
         <v>GRB050525002</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="6">
         <v>41428.659189814818</v>
       </c>
-      <c r="K3" s="1" t="str">
+      <c r="K3" t="str">
         <f t="shared" si="4"/>
         <v>659</v>
       </c>
-      <c r="L3" s="7" t="str">
+      <c r="L3" t="str">
         <f t="shared" ref="L3:L8" si="8">_xlfn.CONCAT(LEFT(I3,LEN(I3)-1), K3)</f>
         <v>GRB130603659</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="6">
         <v>40821.336967592593</v>
       </c>
-      <c r="O3" s="1" t="str">
+      <c r="O3" t="str">
         <f t="shared" si="5"/>
         <v>336</v>
       </c>
-      <c r="P3" s="7" t="str">
+      <c r="P3" t="str">
         <f>_xlfn.CONCAT(LEFT(M3,LEN(M3)-1), O3)</f>
         <v>GRB111005336</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="6">
         <v>38588.966855416664</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>966</v>
       </c>
-      <c r="D4" s="7" t="str">
+      <c r="D4" t="str">
         <f>_xlfn.CONCAT(LEFT(A4,LEN(A4)), C4)</f>
         <v>GRB050824966</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="6">
         <v>42005.641371180558</v>
       </c>
-      <c r="K4" s="1" t="str">
+      <c r="K4" t="str">
         <f t="shared" si="4"/>
         <v>641</v>
       </c>
-      <c r="L4" s="7" t="str">
+      <c r="L4" t="str">
         <f t="shared" si="8"/>
         <v>GRB150101641</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="6">
         <v>40972.248469675927</v>
       </c>
-      <c r="O4" s="1" t="str">
+      <c r="O4" t="str">
         <f t="shared" si="5"/>
         <v>248</v>
       </c>
-      <c r="P4" s="7" t="str">
+      <c r="P4" t="str">
         <f t="shared" ref="P4:P6" si="9">_xlfn.CONCAT(LEFT(M4,LEN(M4)-1), O4)</f>
         <v>GRB120304248</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="6">
         <v>38766.148958333331</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>148</v>
       </c>
-      <c r="D5" s="7" t="str">
+      <c r="D5" t="str">
         <f>_xlfn.CONCAT(LEFT(A5,LEN(A5)), C5)</f>
         <v>GRB060218148</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="6">
         <v>42545.477094907408</v>
       </c>
-      <c r="K5" s="1" t="str">
+      <c r="K5" t="str">
         <f t="shared" si="4"/>
         <v>477</v>
       </c>
-      <c r="L5" s="7" t="str">
+      <c r="L5" t="str">
         <f t="shared" si="8"/>
         <v>GRB160624477</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="6">
         <v>44541.54859953704</v>
       </c>
-      <c r="O5" s="1" t="str">
+      <c r="O5" t="str">
         <f t="shared" si="5"/>
         <v>548</v>
       </c>
-      <c r="P5" s="7" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="9"/>
         <v>GRB211211548</v>
       </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="6">
         <v>38927.800335648149</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="D6" s="7" t="str">
+      <c r="D6" t="str">
         <f>_xlfn.CONCAT(LEFT(A6,LEN(A6)), C6)</f>
         <v>GRB060729800</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="6">
         <v>42603.936956018515</v>
       </c>
-      <c r="K6" s="1" t="str">
+      <c r="K6" t="str">
         <f t="shared" si="4"/>
         <v>936</v>
       </c>
-      <c r="L6" s="7" t="str">
+      <c r="L6" t="str">
         <f t="shared" si="8"/>
         <v>GRB160821936</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="6">
         <v>44992.655624999999</v>
       </c>
-      <c r="O6" s="1" t="str">
+      <c r="O6" t="str">
         <f t="shared" si="5"/>
         <v>655</v>
       </c>
-      <c r="P6" s="7" t="str">
+      <c r="P6" t="str">
         <f t="shared" si="9"/>
         <v>GRB230307655</v>
       </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="6">
         <v>38964.104895833334</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="D7" s="7" t="str">
+      <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>GRB060904104</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="6">
         <v>42964.528541666667</v>
       </c>
-      <c r="K7" s="1" t="str">
+      <c r="K7" t="str">
         <f t="shared" si="4"/>
         <v>528</v>
       </c>
-      <c r="L7" s="7" t="str">
+      <c r="L7" t="str">
         <f t="shared" si="8"/>
         <v>GRB170817528</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="6">
         <v>39191.447280092594</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>447</v>
       </c>
-      <c r="D8" s="7" t="str">
+      <c r="D8" t="str">
         <f t="shared" si="1"/>
         <v>GRB070419447</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="6">
         <v>43973.487199074072</v>
       </c>
-      <c r="K8" s="1" t="str">
+      <c r="K8" t="str">
         <f t="shared" si="4"/>
         <v>487</v>
       </c>
-      <c r="L8" s="7" t="str">
+      <c r="L8" t="str">
         <f t="shared" si="8"/>
         <v>GRB200522487</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="6">
         <v>39380.172847222224</v>
       </c>
-      <c r="C9" s="1" t="str">
+      <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>172</v>
       </c>
-      <c r="D9" s="7" t="str">
+      <c r="D9" t="str">
         <f>_xlfn.CONCAT(LEFT(A9,LEN(A9)), C9)</f>
         <v>GRB071025172</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="6">
         <v>39398.772881944446</v>
       </c>
-      <c r="C10" s="1" t="str">
+      <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>772</v>
       </c>
-      <c r="D10" s="7" t="str">
+      <c r="D10" t="str">
         <f t="shared" si="1"/>
         <v>GRB071112772</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="6">
         <v>39526.258900462963</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>258</v>
       </c>
-      <c r="D11" s="7" t="str">
+      <c r="D11" t="str">
         <f t="shared" si="1"/>
         <v>GRB080319258</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="6">
         <v>39728.224907407406</v>
       </c>
-      <c r="C12" s="1" t="str">
+      <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>224</v>
       </c>
-      <c r="D12" s="7" t="str">
+      <c r="D12" t="str">
         <f>_xlfn.CONCAT(LEFT(A12,LEN(A12)), C12)</f>
         <v>GRB081007224</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="6">
         <v>39982.353113425925</v>
       </c>
-      <c r="C13" s="1" t="str">
+      <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>353</v>
       </c>
-      <c r="D13" s="7" t="str">
+      <c r="D13" t="str">
         <f>_xlfn.CONCAT(LEFT(A13,LEN(A13)), C13)</f>
         <v>GRB090618353</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="6">
         <v>40144.976215277777</v>
       </c>
-      <c r="C14" s="1" t="str">
+      <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>976</v>
       </c>
-      <c r="D14" s="7" t="str">
+      <c r="D14" t="str">
         <f>_xlfn.CONCAT(LEFT(A14,LEN(A14)), C14)</f>
         <v>GRB091127976</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="6">
         <v>40253.531134259261</v>
       </c>
-      <c r="C15" s="1" t="str">
+      <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>531</v>
       </c>
-      <c r="D15" s="7" t="str">
+      <c r="D15" t="str">
         <f t="shared" si="1"/>
         <v>GRB100316531</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="6">
         <v>40286.882037037038</v>
       </c>
-      <c r="C16" s="1" t="str">
+      <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>882</v>
       </c>
-      <c r="D16" s="7" t="str">
+      <c r="D16" t="str">
         <f t="shared" si="1"/>
         <v>GRB100418882</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="6">
         <v>40531.686030092591</v>
       </c>
-      <c r="C17" s="1" t="str">
+      <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>686</v>
       </c>
-      <c r="D17" s="7" t="str">
+      <c r="D17" t="str">
         <f t="shared" si="1"/>
         <v>GRB101219686</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="6">
         <v>40537.77621527778</v>
       </c>
-      <c r="C18" s="1" t="str">
+      <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>776</v>
       </c>
-      <c r="D18" s="7" t="str">
+      <c r="D18" t="str">
         <f t="shared" si="1"/>
         <v>GRB101225776</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="6">
         <v>40886.300092592595</v>
       </c>
-      <c r="C19" s="1" t="str">
+      <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="D19" s="7" t="str">
+      <c r="D19" t="str">
         <f t="shared" si="1"/>
         <v>GRB111209300</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="6">
         <v>40888.928854166668</v>
       </c>
-      <c r="C20" s="1" t="str">
+      <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>928</v>
       </c>
-      <c r="D20" s="7" t="str">
+      <c r="D20" t="str">
         <f t="shared" si="1"/>
         <v>GRB111211928</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="6">
         <v>40905.656053240738</v>
       </c>
-      <c r="C21" s="1" t="str">
+      <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v>656</v>
       </c>
-      <c r="D21" s="7" t="str">
+      <c r="D21" t="str">
         <f t="shared" si="1"/>
         <v>GRB111228656</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="6">
         <v>41021.300034722219</v>
       </c>
-      <c r="C22" s="1" t="str">
+      <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="D22" s="7" t="str">
+      <c r="D22" t="str">
         <f t="shared" si="1"/>
         <v>GRB120422300</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="6">
         <v>41104.888039004632</v>
       </c>
-      <c r="C23" s="1" t="str">
+      <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>888</v>
       </c>
-      <c r="D23" s="7" t="str">
+      <c r="D23" t="str">
         <f t="shared" si="1"/>
         <v>GRB120714888</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="6">
         <v>41119.455717592595</v>
       </c>
-      <c r="C24" s="1" t="str">
+      <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>455</v>
       </c>
-      <c r="D24" s="7" t="str">
+      <c r="D24" t="str">
         <f t="shared" si="1"/>
         <v>GRB120729455</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="6">
         <v>41320.06354166667</v>
       </c>
-      <c r="C25" s="1" t="str">
+      <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>063</v>
       </c>
-      <c r="D25" s="7" t="str">
+      <c r="D25" t="str">
         <f t="shared" si="1"/>
         <v>GRB130215063</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="6">
         <v>41391.324965277781</v>
       </c>
-      <c r="C26" s="1" t="str">
+      <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>324</v>
       </c>
-      <c r="D26" s="7" t="str">
+      <c r="D26" t="str">
         <f t="shared" si="1"/>
         <v>GRB130427324</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="6">
         <v>41457.003739340274</v>
       </c>
-      <c r="C27" s="1" t="str">
+      <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>003</v>
       </c>
-      <c r="D27" s="7" t="str">
+      <c r="D27" t="str">
         <f t="shared" si="1"/>
         <v>GRB130702003</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="6">
         <v>41517.544629629629</v>
       </c>
-      <c r="C28" s="1" t="str">
+      <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>544</v>
       </c>
-      <c r="D28" s="7" t="str">
+      <c r="D28" t="str">
         <f t="shared" si="1"/>
         <v>GRB130831544</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="6">
         <v>41676.303703703707</v>
       </c>
-      <c r="C29" s="1" t="str">
+      <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>303</v>
       </c>
-      <c r="D29" s="7" t="str">
+      <c r="D29" t="str">
         <f t="shared" si="1"/>
         <v>GRB140206303</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="6">
         <v>41796.133239120369</v>
       </c>
-      <c r="C30" s="1" t="str">
+      <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>133</v>
       </c>
-      <c r="D30" s="7" t="str">
+      <c r="D30" t="str">
         <f t="shared" si="1"/>
         <v>GRB140606133</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="6">
         <v>42234.483703703707</v>
       </c>
-      <c r="C31" s="1" t="str">
+      <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>483</v>
       </c>
-      <c r="D31" s="7" t="str">
+      <c r="D31" t="str">
         <f t="shared" si="1"/>
         <v>GRB150818483</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="6">
         <v>42723.783784722225</v>
       </c>
-      <c r="C32" s="1" t="str">
+      <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v>783</v>
       </c>
-      <c r="D32" s="7" t="str">
+      <c r="D32" t="str">
         <f t="shared" si="1"/>
         <v>GRB161219783</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="6">
         <v>42732.552567673614</v>
       </c>
-      <c r="C33" s="1" t="str">
+      <c r="C33" t="str">
         <f t="shared" si="0"/>
         <v>552</v>
       </c>
-      <c r="D33" s="7" t="str">
+      <c r="D33" t="str">
         <f t="shared" si="1"/>
         <v>GRB161228552</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="6">
         <v>43018.792252083331</v>
       </c>
-      <c r="C34" s="1" t="str">
+      <c r="C34" t="str">
         <f t="shared" si="0"/>
         <v>792</v>
       </c>
-      <c r="D34" s="7" t="str">
+      <c r="D34" t="str">
         <f t="shared" si="1"/>
         <v>GRB171010792</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="6">
         <v>43074.30605324074</v>
       </c>
-      <c r="C35" s="1" t="str">
+      <c r="C35" t="str">
         <f t="shared" si="0"/>
         <v>306</v>
       </c>
-      <c r="D35" s="7" t="str">
+      <c r="D35" t="str">
         <f t="shared" si="1"/>
         <v>GRB171205306</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="6">
         <v>43301.598425925928</v>
       </c>
-      <c r="C36" s="1" t="str">
+      <c r="C36" t="str">
         <f t="shared" si="0"/>
         <v>598</v>
       </c>
-      <c r="D36" s="7" t="str">
+      <c r="D36" t="str">
         <f t="shared" si="1"/>
         <v>GRB180720598</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="6">
         <v>43309.728472222225</v>
       </c>
-      <c r="C37" s="1" t="str">
+      <c r="C37" t="str">
         <f t="shared" si="0"/>
         <v>728</v>
       </c>
-      <c r="D37" s="7" t="str">
+      <c r="D37" t="str">
         <f t="shared" si="1"/>
         <v>GRB180728728</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="6">
         <v>43479.87295138889</v>
       </c>
-      <c r="C38" s="1" t="str">
+      <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v>872</v>
       </c>
-      <c r="D38" s="7" t="str">
+      <c r="D38" t="str">
         <f t="shared" si="1"/>
         <v>GRB190114872</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="6">
         <v>43706.830474537041</v>
       </c>
-      <c r="C39" s="1" t="str">
+      <c r="C39" t="str">
         <f>LEFT(RIGHT(B39,LEN(B39)-FIND(".",B39)),3)</f>
         <v>830</v>
       </c>
-      <c r="D39" s="7" t="str">
+      <c r="D39" t="str">
         <f>_xlfn.CONCAT(LEFT(A39,LEN(A39)-1), C39)</f>
         <v>GRB190829830</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="6">
         <v>44069.187407407408</v>
       </c>
-      <c r="C40" s="1" t="str">
+      <c r="C40" t="str">
         <f t="shared" ref="C40:C42" si="10">LEFT(RIGHT(B40,LEN(B40)-FIND(".",B40)),3)</f>
         <v>187</v>
       </c>
-      <c r="D40" s="7" t="str">
+      <c r="D40" t="str">
         <f t="shared" ref="D40:D43" si="11">_xlfn.CONCAT(LEFT(A40,LEN(A40)-1), C40)</f>
         <v>GRB200826187</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="6">
         <v>44237.083645833336</v>
       </c>
-      <c r="C41" s="1" t="str">
+      <c r="C41" t="str">
         <f t="shared" si="10"/>
         <v>083</v>
       </c>
-      <c r="D41" s="7" t="str">
+      <c r="D41" t="str">
         <f t="shared" si="11"/>
         <v>GRB210210083</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="6">
         <v>44492.545636574076</v>
       </c>
-      <c r="C42" s="1" t="str">
+      <c r="C42" t="str">
         <f t="shared" si="10"/>
         <v>545</v>
       </c>
-      <c r="D42" s="7" t="str">
+      <c r="D42" t="str">
         <f t="shared" si="11"/>
         <v>GRB211023545</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="6">
         <v>44843.553460648145</v>
       </c>
-      <c r="C43" s="1" t="str">
+      <c r="C43" t="str">
         <f>LEFT(RIGHT(B43,LEN(B43)-FIND(".",B43)),3)</f>
         <v>553</v>
       </c>
-      <c r="D43" s="7" t="str">
+      <c r="D43" t="str">
         <f t="shared" si="11"/>
         <v>GRB221009553</v>
       </c>

</xml_diff>